<commit_message>
Added Course Name for each Coupon in excel
</commit_message>
<xml_diff>
--- a/CouponsData.xlsx
+++ b/CouponsData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,211 +448,361 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/nlp-with-transformers/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-8_TKEVmD148SLcYn9Lwr0w&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREE43</t>
+          <t>https://www.udemy.com/course/full-stack-programming-for-complete-beginners-in-python/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-gIbnrEzx9KRq46QVSLoN5w&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEAGAIN2</t>
         </is>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/fundamental-question-on-industrial-electronics/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-2jcaES8HGbMyKcOoyh4owA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=03476819394E431897AD</t>
+          <t>https://www.udemy.com/course/bootstrap-5-with-5-projects-in-hindi-urdu/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-FvQ_.CTp0rL1vTOF2Xk75w&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEBOOTSTRAP5</t>
         </is>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/certified-kubernetes-administrator-cka-practice-exams-2021-g/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-KftDcNRdbkLXV7Y.W89ouQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
+          <t>https://www.udemy.com/course/jenkins-github-and-aws-in-practice/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-T9l1LjEiqk1DtyQUZ0MRDQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=TAPIR4U</t>
         </is>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/aws-certified-security-specialty-practice-exams-latest-2021/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-mS4cQT2kgrkwCTWPhJf3pw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
+          <t>https://www.udemy.com/course/nlp-with-transformers/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-8_TKEVmD148SLcYn9Lwr0w&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREE43</t>
         </is>
       </c>
       <c r="B5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/introduction-to-forex-learn-to-trade-forex-by-yourself/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-YlmLkeHLGgDClMVe_x35Mg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=90B03C13055C47A28233</t>
+          <t>https://www.udemy.com/course/fundamental-question-on-industrial-electronics/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-2jcaES8HGbMyKcOoyh4owA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=03476819394E431897AD</t>
         </is>
       </c>
       <c r="B6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/the-complete-introduction-to-the-deep-web/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-ejoNkDbidMtJkVt3Dik03g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=BFEF8CEA0D5C02B295EC</t>
+          <t>https://www.udemy.com/course/certified-kubernetes-administrator-cka-practice-exams-2021-g/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-KftDcNRdbkLXV7Y.W89ouQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
         </is>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/java-programming-complete-beginner-to-advanced/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-kFna2ZPAJFIvysrg1IHSXQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=657F843318F537</t>
+          <t>https://www.udemy.com/course/aws-certified-security-specialty-practice-exams-latest-2021/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-mS4cQT2kgrkwCTWPhJf3pw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
         </is>
       </c>
       <c r="B8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/learn-guitar/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-7v0f5KRpF9pOzWBLcs4awg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEMAY2021</t>
+          <t>https://www.udemy.com/course/introduction-to-forex-learn-to-trade-forex-by-yourself/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-YlmLkeHLGgDClMVe_x35Mg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=90B03C13055C47A28233</t>
         </is>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/mathematics-software-development/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-4bG5mVFPyenfGx9DIxxGqg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=716CB1EDFA7A3BDBA012</t>
+          <t>https://www.udemy.com/course/the-complete-introduction-to-the-deep-web/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-ejoNkDbidMtJkVt3Dik03g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=BFEF8CEA0D5C02B295EC</t>
         </is>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/learn-html5-in-depth-with-real-world-examples/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-TiBjtkhZWAdnGjFKUfXeYA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREE-JUNE</t>
+          <t>https://www.udemy.com/course/java-programming-complete-beginner-to-advanced/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-kFna2ZPAJFIvysrg1IHSXQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=657F843318F537</t>
         </is>
       </c>
       <c r="B11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/five-proven-steps-to-real-estate-investing-success/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-xiCN6r1IgPMk4R7tTpCC0A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FPSREEXPJUNE72021</t>
+          <t>https://www.udemy.com/course/learn-guitar/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-7v0f5KRpF9pOzWBLcs4awg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEMAY2021</t>
         </is>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/css3-in-hindi/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-8glOs2QMsLJlDbNfDfnc1A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEHTML</t>
+          <t>https://www.udemy.com/course/mathematics-software-development/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-4bG5mVFPyenfGx9DIxxGqg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=716CB1EDFA7A3BDBA012</t>
         </is>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/the-complete-nft-non-fungible-tokens-course-for-artists/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-z8Qt6L.JD4drRJYzQBiIbA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=C31651B940736748184A</t>
+          <t>https://www.udemy.com/course/learn-html5-in-depth-with-real-world-examples/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-TiBjtkhZWAdnGjFKUfXeYA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREE-JUNE</t>
         </is>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/criminology-fundamentals-of-criminal-psychology-and-law/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-_w5DXJ__glaVUmoWmPyr_g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=TECHBINZ</t>
+          <t>https://www.udemy.com/course/five-proven-steps-to-real-estate-investing-success/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-xiCN6r1IgPMk4R7tTpCC0A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FPSREEXPJUNE72021</t>
         </is>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/malware-analysis-of-documents/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-M60CuswLMGrVodxClHsuyw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FMADFREE_JUN2</t>
+          <t>https://www.udemy.com/course/css3-in-hindi/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-8glOs2QMsLJlDbNfDfnc1A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEHTML</t>
         </is>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/togaf-9-practice-exams-2021-combined-level-1-and-2/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-V6Bt8vkXdVJ_Rt7f.0ZX0A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
+          <t>https://www.udemy.com/course/the-complete-nft-non-fungible-tokens-course-for-artists/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-z8Qt6L.JD4drRJYzQBiIbA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=C31651B940736748184A</t>
         </is>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/nestjs-zero-to-hero/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-vuix.OYJdweFzxNEc4xWJA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=JUNE_REPRODUCTION</t>
+          <t>https://www.udemy.com/course/criminology-fundamentals-of-criminal-psychology-and-law/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-_w5DXJ__glaVUmoWmPyr_g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=TECHBINZ</t>
         </is>
       </c>
       <c r="B18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/powerbi-hero/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-fSCXMHSvvdOYIAtMa0V.CQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDASHBI</t>
+          <t>https://www.udemy.com/course/malware-analysis-of-documents/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-M60CuswLMGrVodxClHsuyw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FMADFREE_JUN2</t>
         </is>
       </c>
       <c r="B19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/pmp-practice-test-project-management-professional-2021/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-3NzgBtrhXZl306P5kOdkQQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=88B2BE4D7ADDB73DC2A8</t>
+          <t>https://www.udemy.com/course/togaf-9-practice-exams-2021-combined-level-1-and-2/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-V6Bt8vkXdVJ_Rt7f.0ZX0A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
         </is>
       </c>
       <c r="B20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/procreate-sketch-draw-and-paint-a-shirt-design/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-Ka.lQqaDDH5LeKmXA62xAA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=479DD8FB85D20883AD98</t>
+          <t>https://www.udemy.com/course/nestjs-zero-to-hero/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-vuix.OYJdweFzxNEc4xWJA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=JUNE_REPRODUCTION</t>
         </is>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>https://www.udemy.com/course/powerbi-hero/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-fSCXMHSvvdOYIAtMa0V.CQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDASHBI</t>
+        </is>
+      </c>
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/pmp-practice-test-project-management-professional-2021/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-3NzgBtrhXZl306P5kOdkQQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=88B2BE4D7ADDB73DC2A8</t>
+        </is>
+      </c>
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/procreate-sketch-draw-and-paint-a-shirt-design/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-Ka.lQqaDDH5LeKmXA62xAA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=479DD8FB85D20883AD98</t>
+        </is>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>https://www.udemy.com/course/certified-ethical-hacker-ceh-v11-practice-exams-new-2021-p/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-C_tWhI4fou94y_Fuhc.GTA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
         </is>
       </c>
-      <c r="B22" t="b">
-        <v>1</v>
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/statistics-with-r-beginner-level/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-wHtlPlYCyDJnSo1Ig1G7sQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=BLIZZARD</t>
+        </is>
+      </c>
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/introduction-to-quantum-computing/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-NwgU.ZGMVqjWDGDnRgRf8w&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=1E58CF6234A770ADB7D4</t>
+        </is>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/internet-and-web-development-fundamentals/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-JA4ZkVqndBxpGFa4FQ_yhA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=YOUACCEL44184</t>
+        </is>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/learn-to-create-ai-voice-assistant-jarvis-with-python/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-XFOMo1r_V.kB_SehUO8kvw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=5B0D13596E86F8590815</t>
+        </is>
+      </c>
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/advanced-neural-networks-in-r-a-practical-approach/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-D1Y2FQMwQso0jlxOpoolDQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=BLIZZARD</t>
+        </is>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/master-complete-statistics-for-computer-science-i/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-5zpyg0CV2g64pUfJxfd3RQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEMCSCS8</t>
+        </is>
+      </c>
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/automate/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-2RAEBfwHARDAqISmMGjr6g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=JUN2021FREE</t>
+        </is>
+      </c>
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/profitable-binary-trading-beginners-guide/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-zJCCLL3oT5a2984mJvElkw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=F38EAFE4B41DC5727483</t>
+        </is>
+      </c>
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/complete-progressive-web-app-bootcamp/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-A9qitzgGelGw6tDMleaNfw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FD68EF3DA859515E0BA4</t>
+        </is>
+      </c>
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/best-sap-fico-tutorial-for-beginners-freshers/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-zM9AA4RsBoUM1evDQAly9Q&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEJUNE</t>
+        </is>
+      </c>
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/applied-ethical-hacking-and-rules-of-engagement/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-uOqvxC2Uedsk38t.dec0nA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=AFFD464DDCD4D7C2AA17</t>
+        </is>
+      </c>
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/complete-linux-command-line-and-terminal-productivity/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-qNlUgfwBDe0d1W_LaYdP8A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=5CAEA2E49267B0A52E44</t>
+        </is>
+      </c>
+      <c r="B37" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scraping Content Changed and fixed error
</commit_message>
<xml_diff>
--- a/CouponsData.xlsx
+++ b/CouponsData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,10 +436,15 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Coupon URL</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>isValid</t>
         </is>
@@ -448,360 +453,892 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/full-stack-programming-for-complete-beginners-in-python/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-gIbnrEzx9KRq46QVSLoN5w&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEAGAIN2</t>
-        </is>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
+          <t>Typescript with React quick start – with Jest testing</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/typescript-with-react-jest-testing/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-OcvUMwnM.1DAnXjb6CiduQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEJUL20213</t>
+        </is>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/bootstrap-5-with-5-projects-in-hindi-urdu/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-FvQ_.CTp0rL1vTOF2Xk75w&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEBOOTSTRAP5</t>
-        </is>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
+          <t>ManageEngine OPManager Plus Network Monitoring Course</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/manageengin-opmanager-network-performance-monitoring-course/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-2Kgs.AVpi2.4JQd2YkeaKQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=48EAB7B94EB06A83F2A2</t>
+        </is>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/jenkins-github-and-aws-in-practice/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-T9l1LjEiqk1DtyQUZ0MRDQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=TAPIR4U</t>
-        </is>
-      </c>
-      <c r="B4" t="b">
-        <v>0</v>
+          <t>Searching and Sorting Algorithms</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/searching-and-sorting-algorithms/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-_uY1c5fCibBrqIHlujlw1Q&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=AB8E834D846589C36490</t>
+        </is>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/nlp-with-transformers/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-8_TKEVmD148SLcYn9Lwr0w&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREE43</t>
-        </is>
-      </c>
-      <c r="B5" t="b">
-        <v>0</v>
+          <t>Learn Spanish Now: All-in-One Knowledge Course</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/learn-spanish-now/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-Pdpwk9LG_4Zp0eOqVkPnRQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=NEWSTUDENT</t>
+        </is>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>https://www.udemy.com/course/fundamental-question-on-industrial-electronics/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-2jcaES8HGbMyKcOoyh4owA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=03476819394E431897AD</t>
-        </is>
-      </c>
-      <c r="B6" t="b">
-        <v>0</v>
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/sensors-interfacing-sensor-wiring-sensor-temperature-humidity-sensors/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-v_LonqJkEOM2NTkLH2pZ2g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=JULYSTAYHOME</t>
+        </is>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/certified-kubernetes-administrator-cka-practice-exams-2021-g/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-KftDcNRdbkLXV7Y.W89ouQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
-        </is>
-      </c>
-      <c r="B7" t="b">
-        <v>0</v>
+          <t>GoF Design Patterns – Complete Course with Java Examples</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/gof-design-patterns-learnit/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-a.acyB1.LNp4OfGiQq5epA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=GOF_JUL_FREE_2</t>
+        </is>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/aws-certified-security-specialty-practice-exams-latest-2021/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-mS4cQT2kgrkwCTWPhJf3pw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
-        </is>
-      </c>
-      <c r="B8" t="b">
+          <t>Complete Korean Course: Learn Korean for Beginners</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/korean-for-complete-beginners/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-c2VS18EzV.ptbHc.z8OnoQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=D865FB5298E6933BC442</t>
+        </is>
+      </c>
+      <c r="C8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/introduction-to-forex-learn-to-trade-forex-by-yourself/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-YlmLkeHLGgDClMVe_x35Mg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=90B03C13055C47A28233</t>
-        </is>
-      </c>
-      <c r="B9" t="b">
+          <t>React JS- Complete Guide for Frontend Web Development [2021]</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/react-js-a-complete-guide-for-frontend-web-development/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-PIdIjtD94iAgr2dQOXgP6Q&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEJULY5</t>
+        </is>
+      </c>
+      <c r="C9" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/the-complete-introduction-to-the-deep-web/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-ejoNkDbidMtJkVt3Dik03g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=BFEF8CEA0D5C02B295EC</t>
-        </is>
-      </c>
-      <c r="B10" t="b">
+          <t>DevOps Fundamentals</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/devops-fundamentals-for-beginners/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-6TmlLrpxu_K5jfssvLPZcA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEJULY5</t>
+        </is>
+      </c>
+      <c r="C10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/java-programming-complete-beginner-to-advanced/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-kFna2ZPAJFIvysrg1IHSXQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=657F843318F537</t>
-        </is>
-      </c>
-      <c r="B11" t="b">
+          <t>The Complete MERN Stack Development course 2021</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/mern-stack-with-blog-project/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-.o.UdiXmhA7EY9c3hErzfg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=8BF0EAF81C8389C3422B</t>
+        </is>
+      </c>
+      <c r="C11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/learn-guitar/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-7v0f5KRpF9pOzWBLcs4awg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEMAY2021</t>
-        </is>
-      </c>
-      <c r="B12" t="b">
+          <t xml:space="preserve"> From Basics to Advanced</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/step-by-step-guide-to-machine-learning-course/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-m71Bj1ahp3v_hXDSSSw7Cw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEJULY5</t>
+        </is>
+      </c>
+      <c r="C12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/mathematics-software-development/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-4bG5mVFPyenfGx9DIxxGqg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=716CB1EDFA7A3BDBA012</t>
-        </is>
-      </c>
-      <c r="B13" t="b">
+          <t>Object-Oriented Programming (OOP) – From Basics to Advance (Java)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/oop-learnit/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-ZoQq3hgvMeYyRNPA2eO6ug&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=OOP_JUL_FREE_2</t>
+        </is>
+      </c>
+      <c r="C13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/learn-html5-in-depth-with-real-world-examples/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-TiBjtkhZWAdnGjFKUfXeYA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREE-JUNE</t>
-        </is>
-      </c>
-      <c r="B14" t="b">
+          <t>Introduction to Java unit testing with JUnit5 framework</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/introduction-to-java-unit-testing-with-junit5-framework/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-B3Du1Z3e9fr68xilbIdwBw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=6FAF3D45B36BC0534B24</t>
+        </is>
+      </c>
+      <c r="C14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/five-proven-steps-to-real-estate-investing-success/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-xiCN6r1IgPMk4R7tTpCC0A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FPSREEXPJUNE72021</t>
-        </is>
-      </c>
-      <c r="B15" t="b">
+          <t>Front End Web Development Ultimate Course 2021</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/learn-front-end-development/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-uh_2vPtAFwx7sVIki5DnnA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=TRY10FREE72105</t>
+        </is>
+      </c>
+      <c r="C15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/css3-in-hindi/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-8glOs2QMsLJlDbNfDfnc1A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEHTML</t>
-        </is>
-      </c>
-      <c r="B16" t="b">
+          <t>Java Programming: Complete Beginner to Advanced</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/java-programming-complete-beginner-to-advanced/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-Aao5AiBjlpgjc1Rz7zAhtw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=D17864248C</t>
+        </is>
+      </c>
+      <c r="C16" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/the-complete-nft-non-fungible-tokens-course-for-artists/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-z8Qt6L.JD4drRJYzQBiIbA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=C31651B940736748184A</t>
-        </is>
-      </c>
-      <c r="B17" t="b">
+          <t>Google Workspace (G Suite) Ultimate Course 2021</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/learn-g-suite/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-ICG164fdUce4DexozQ04Ag&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=TRY10FREE72105</t>
+        </is>
+      </c>
+      <c r="C17" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/criminology-fundamentals-of-criminal-psychology-and-law/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-_w5DXJ__glaVUmoWmPyr_g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=TECHBINZ</t>
-        </is>
-      </c>
-      <c r="B18" t="b">
+          <t>Python 3 Master Course for 2021</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/python-3-master-course-for-2021/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-8GPz5cf8Uj9RMe13v.2JQA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=TRY10FREE72105</t>
+        </is>
+      </c>
+      <c r="C18" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/malware-analysis-of-documents/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-M60CuswLMGrVodxClHsuyw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FMADFREE_JUN2</t>
-        </is>
-      </c>
-      <c r="B19" t="b">
+          <t>Complete Graphics Design and Video Editing Masterclass</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/complete-graphics-design-and-video-editing-masterclass/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-VBUUvMSDxN.LEfiGitjtFw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=MASTERCLASS_FREE</t>
+        </is>
+      </c>
+      <c r="C19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>https://www.udemy.com/course/togaf-9-practice-exams-2021-combined-level-1-and-2/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-V6Bt8vkXdVJ_Rt7f.0ZX0A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
-        </is>
-      </c>
-      <c r="B20" t="b">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/quantitative-aptitude-for-cat/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-Ui6q65ndkcGCvqDY8xyPjw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=SUBHA386</t>
+        </is>
+      </c>
+      <c r="C20" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/nestjs-zero-to-hero/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-vuix.OYJdweFzxNEc4xWJA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=JUNE_REPRODUCTION</t>
-        </is>
-      </c>
-      <c r="B21" t="b">
+          <t>The Complete High School and College Mathematics</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/the-complete-high-school-and-college-mathematics/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-dxAVxkPsyFO.C7MVrxp9lg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEJULY</t>
+        </is>
+      </c>
+      <c r="C21" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/powerbi-hero/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-fSCXMHSvvdOYIAtMa0V.CQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDASHBI</t>
-        </is>
-      </c>
-      <c r="B22" t="b">
+          <t>Programming Network Applications in Java</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/programming-network-applications-in-java/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-3TbMH2zybOLLKtNiL2ygpw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=JULY21FREE</t>
+        </is>
+      </c>
+      <c r="C22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/pmp-practice-test-project-management-professional-2021/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-3NzgBtrhXZl306P5kOdkQQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=88B2BE4D7ADDB73DC2A8</t>
-        </is>
-      </c>
-      <c r="B23" t="b">
+          <t>The Complete SAP Analytics Cloud Course 2021</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/sap-analytics-cloud-sac/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-56hQJVKYnLH6QwMOcGbIow&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=9C9CE3340CFD8AFCEDF2</t>
+        </is>
+      </c>
+      <c r="C23" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/procreate-sketch-draw-and-paint-a-shirt-design/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-Ka.lQqaDDH5LeKmXA62xAA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=479DD8FB85D20883AD98</t>
-        </is>
-      </c>
-      <c r="B24" t="b">
+          <t>XSS Survival Guide</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/xss-survival-guide/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-UAZcXGsure4qvzkKy_VWRA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=E820801EC6E03485F241</t>
+        </is>
+      </c>
+      <c r="C24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/certified-ethical-hacker-ceh-v11-practice-exams-new-2021-p/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-C_tWhI4fou94y_Fuhc.GTA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDAYS</t>
-        </is>
-      </c>
-      <c r="B25" t="b">
+          <t>Learn Bootstrap – For Beginners</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/learn-bootstrap-for-beginners/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-EKLT5oO0mOPXQgcC4n452g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=YOUACCEL46587</t>
+        </is>
+      </c>
+      <c r="C25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/statistics-with-r-beginner-level/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-wHtlPlYCyDJnSo1Ig1G7sQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=BLIZZARD</t>
-        </is>
-      </c>
-      <c r="B26" t="b">
+          <t>Master Python With NumPy For Data Science and Machine Learning</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/numpy-for-data-science-and-machine-learning/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-Goz6j1P00.TTDMVQrriRhA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=446B7A7BE0A314A94427</t>
+        </is>
+      </c>
+      <c r="C26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/introduction-to-quantum-computing/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-NwgU.ZGMVqjWDGDnRgRf8w&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=1E58CF6234A770ADB7D4</t>
-        </is>
-      </c>
-      <c r="B27" t="b">
+          <t>Complete JAVASCRIPT with HTML5,CSS3 from zero to Expert-2021</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/build-responsive-website-using-html5-css3-js-and-bootstrap-p/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-7pnEfoop.MrhkvMdXydwKw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=4D07D2277F23DC426AC0</t>
+        </is>
+      </c>
+      <c r="C27" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/internet-and-web-development-fundamentals/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-JA4ZkVqndBxpGFa4FQ_yhA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=YOUACCEL44184</t>
-        </is>
-      </c>
-      <c r="B28" t="b">
+          <t>Complete Italian Course: Learn Italian for Beginners Level 1</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/complete-italian-course/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-vFuIbVykDobKp2YIEzaHtg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=93C51DC334A1533ACDF4</t>
+        </is>
+      </c>
+      <c r="C28" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/learn-to-create-ai-voice-assistant-jarvis-with-python/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-XFOMo1r_V.kB_SehUO8kvw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=5B0D13596E86F8590815</t>
-        </is>
-      </c>
-      <c r="B29" t="b">
+          <t>SVG Ultimate Course</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/learn-advanced-svg/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-7ctvE9.vpJN6q08IJeeFiQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=TRY10FREE62107</t>
+        </is>
+      </c>
+      <c r="C29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/advanced-neural-networks-in-r-a-practical-approach/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-D1Y2FQMwQso0jlxOpoolDQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=BLIZZARD</t>
-        </is>
-      </c>
-      <c r="B30" t="b">
+          <t>Python Network Programming for Network Engineers (Python 3)</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/python-network-programming-for-network-engineers-python-3/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-GtuAnU4nCrTIMwm.NfZrcg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=JUNE22</t>
+        </is>
+      </c>
+      <c r="C30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/master-complete-statistics-for-computer-science-i/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-5zpyg0CV2g64pUfJxfd3RQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEMCSCS8</t>
-        </is>
-      </c>
-      <c r="B31" t="b">
+          <t>2021 Complete Pyomo Bootcamp: Python Optimization Beginners</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/optimization-in-python/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-HwTArAJbQAET9INwAwPd.w&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEPYOMO</t>
+        </is>
+      </c>
+      <c r="C31" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/automate/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-2RAEBfwHARDAqISmMGjr6g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=JUN2021FREE</t>
-        </is>
-      </c>
-      <c r="B32" t="b">
+          <t>Wireshark: Packet Analysis and Ethical Hacking: Core Skills</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/wireshark-packet-analysis-and-ethical-hacking-core-skills/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-DdYVvI2zokei8Yupx1ozpg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=JUNE22</t>
+        </is>
+      </c>
+      <c r="C32" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/profitable-binary-trading-beginners-guide/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-zJCCLL3oT5a2984mJvElkw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=F38EAFE4B41DC5727483</t>
-        </is>
-      </c>
-      <c r="B33" t="b">
+          <t>Everything About Blogger From Scratch</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/rkeverything-about-blogger-from-scratch/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-TDZJl3kA7nlkRuXxcc9VZQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=76A71B1901F5A33AE3A6</t>
+        </is>
+      </c>
+      <c r="C33" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/complete-progressive-web-app-bootcamp/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-A9qitzgGelGw6tDMleaNfw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FD68EF3DA859515E0BA4</t>
-        </is>
-      </c>
-      <c r="B34" t="b">
+          <t>Ultimate TallyPrime With GST Step By Step Guide – 2021</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/ultimate-tallyprime-with-gst-step-by-step-guide-2021/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-mAp6UjuQNFidpALtImXovA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=TRICKYMAN</t>
+        </is>
+      </c>
+      <c r="C34" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/best-sap-fico-tutorial-for-beginners-freshers/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-zM9AA4RsBoUM1evDQAly9Q&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEJUNE</t>
-        </is>
-      </c>
-      <c r="B35" t="b">
+          <t>Advanced Microsoft Excel Formulas &amp; Functions Course 2021</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/advanced-microsoft-excel-formulas-functions/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-hjjqwEugmUfBZ7c07PKkBA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads</t>
+        </is>
+      </c>
+      <c r="C35" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/applied-ethical-hacking-and-rules-of-engagement/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-uOqvxC2Uedsk38t.dec0nA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=AFFD464DDCD4D7C2AA17</t>
-        </is>
-      </c>
-      <c r="B36" t="b">
+          <t>Intro To Adobe Color, Spark, Rush, &amp; Bandlab</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/intro-to-adobe-color-spark-photoshop-express-editor/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-nnL.qUZD91cysybcM0sviA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=B0CE6E6C0D2D1EB96F37</t>
+        </is>
+      </c>
+      <c r="C36" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.udemy.com/course/complete-linux-command-line-and-terminal-productivity/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-qNlUgfwBDe0d1W_LaYdP8A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=5CAEA2E49267B0A52E44</t>
-        </is>
-      </c>
-      <c r="B37" t="b">
+          <t>C++ Programming Step By Step From Beginner To Ultimate Level</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/c-programming-step-by-step-from-beginner-to-ultimate-level/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-3rn6K.B.NwHdQg7jksAAtA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=44C5196B9A75A4CA2D65</t>
+        </is>
+      </c>
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Linux / Unix For Beginners</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/linux-unix-for-beginners/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-fqDiwq75HLIuFUV7GZjFzw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=HURRY4U</t>
+        </is>
+      </c>
+      <c r="C38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Drupal For Absolute Beginners (2021)</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/drupal-masterclass/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-I4IQZMP3TzglCFtIZo4D5g&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=534ECDD47F178A737B43</t>
+        </is>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>API Crash Course: What is an API, how to create it and test it</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/api-course/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-.MjC9nN_OglorT.7jm4Qhw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=A8ACD96D71618FB5E347</t>
+        </is>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Unity C# 2d- Memory Matching Game</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/unity2d-memory-matching-game/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-_fpPS5FpXI0.t6a9TrUKZA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=F19B0399445D690B3952</t>
+        </is>
+      </c>
+      <c r="C41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Game Development with PyGame | Real World Games</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/pygame-python/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-XhoYcJd7GKY_eUTxhgVFCg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=79773A85F8F706BEC7D2</t>
+        </is>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Build A Custom Dynamic Blog Website with PHP, MySQL and Jquery</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/build-a-blog-website/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-D6B8_VLuxRTwta79umsmPA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREECOURSE</t>
+        </is>
+      </c>
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Graphic Design – Passive Income Downloads and Self Publishing</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/graphic-design-passive-income-downloads-self-publishing/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-a6NE7m3MbghxW2jZD2PDWw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=12BAAF6D0C6370EC39BB</t>
+        </is>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Complete WordPress Website Developer Course</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/the-complete-wordpress-developer-course-w/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-ESzD1XV9YzL8RHVtSFB7tA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=2709E0C8D3965EB37BDA</t>
+        </is>
+      </c>
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Ultimate Beginner Guide to Streamlabs OBS (SlOBS)</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/ultimate-beginner-guide-for-streamlabs-obs/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-3Y2WrIkK.jmEeWy6Xlu81A&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=E381D6E2663E6DD6599D</t>
+        </is>
+      </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>.NET Core Web API, Vue JS &amp; Microsoft SQL Full-Stack Web App</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/dot-net-core-web-api-vue-js-microsoft-sql-full-stack-web-app/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-eapYzd7RalWQ3w89dl1Lcw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=5B6A26B235D182F77316</t>
+        </is>
+      </c>
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Complete Filipino Course: Learn Filipino for Beginners</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/complete-filipino-course-learn-tagalog-for-beginners/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-Zqye0uiMf0YcsRVa5q7auw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=618A71E3B9D84692D4BD</t>
+        </is>
+      </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>PhpStorm master class. The best php IDE for fullstack dev</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/phpstorm-masterclass-best-php-ide-fullstack-laravel-angular-react/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-qsm9h9RCo5EqG9KS6EssLA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=LEARNPHPSTORM</t>
+        </is>
+      </c>
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Broad Scope Bug Bounties From Scratch</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/broad-scope-bug-bounties-from-scratch/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-XpqEwUgW4YYbwXshcUpUKw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=9943A2D06E764688003B</t>
+        </is>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Advanced Data Analytics Training using Python</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/data-analytics-python/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-D439XM3y5zxxjGrBI.tpNQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=BIGTREAT</t>
+        </is>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Tableau Certified Associate Certification Exam Prep 2021</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/tableau_certified_associate/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-yvB.ZTuzbd7Or2dV5eR9aQ&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREE2021</t>
+        </is>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>OBS Studio – Ultimate Livestreaming Guide to OBS Studio</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/ultimate-beginners-guide-to-open-broadcaster-softwareobs/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-IrqjE5sn5cT2mX3rV3zogA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=1C2E68366A36A4E5DBD1</t>
+        </is>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Python for Data Science</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/top-python-for-data-science-course/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-PysF6d0XtQM6n3PJRAsIgg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=PYTHON100</t>
+        </is>
+      </c>
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Machine Learning using Python Programming</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/machine-learning-using-python-programming/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-hlIsAOCj2OqorYxmEg4EzA&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=MACHINE_LEARNING</t>
+        </is>
+      </c>
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Beginner English: Practical Foundational English Training</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/beginner-english-esl/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-TmpBxbyIK8ZAQlKmGqyYSw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=BEPFEEXPJUNE242021</t>
+        </is>
+      </c>
+      <c r="C56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>The Complete React Redux Node Express MySQL Developer Course</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/the-complete-react-redux-node-express-mysql-developer-course/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-lKA8nfNBWyENF.Hu7vyYLg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=C8900A8D8FF555898E9B</t>
+        </is>
+      </c>
+      <c r="C57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>The SQL MicroDegree 2021: From SQL Basics To Advanced SQL</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/sqlmicrodegree/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-Zj6E_2vQJe0unrw.jjxTeg&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEMICRODEGREE</t>
+        </is>
+      </c>
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Digital Marketing Strategy 2021. Start from scratch!</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/digital-marketing-strategy-from-scratch-course/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-J5UuQjFe0B3XEiNKfDZEQw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=FREEDIGITALSUMMER</t>
+        </is>
+      </c>
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Advance Bug Bounty Hunting and Penetration Testing Course 2021</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/advance-bug-bounty-hunting-penetration-testing-course-2021/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-3z6TvqXhiBTPS7a5pHpkow&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=722CD85698BF5D8E5B64</t>
+        </is>
+      </c>
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Learn to Host Multiple Domains on one Virtual Server</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>https://www.udemy.com/course/learn-to-host-multiple-domains-on-one-virtual-server/?ranMID=39197&amp;ranEAID=%2F7fFXpljNdk&amp;ranSiteID=_7fFXpljNdk-cmwu8eEJ3_rS8qfFmyakyw&amp;LSNPUBID=%2F7fFXpljNdk&amp;utm_source=aff-campaign&amp;utm_medium=udemyads&amp;couponCode=YOUACCEL40602</t>
+        </is>
+      </c>
+      <c r="C61" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>